<commit_message>
atualizacao do mapeamento de ambientes das app Non-SAP
</commit_message>
<xml_diff>
--- a/Test Enviroment Plan V4.xlsx
+++ b/Test Enviroment Plan V4.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="149">
   <si>
     <t>PnS</t>
   </si>
@@ -434,10 +434,6 @@
   </si>
   <si>
     <t xml:space="preserve"> \\BRSPTEST01\CredRuralPF17\CCredRural\CR.accdb</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> http://brsptestpf17/cartoesvisita/
- http://brsptestpf17/sgdi_new/</t>
   </si>
   <si>
     <t xml:space="preserve"> http://brspwproj14:7979/pricingspot
@@ -515,6 +511,20 @@
 db: db_synseg
 SSIS_RepositorioSAPRH_CargaTXT (job mesmo nome)
 SSIS_Atualiza_Repositorio_BRSPSQL03 ((job mesmo nome))</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://brsptest01/cartoesvisitauat/
+ http://brsptest01/sgdi_new_uat/
+SQL instance: brsptest01\sqlserver2012
+db=CartaoVisita
+db=sgdi_new</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> http://brsptestpf17/cartoesvisita/
+ http://brsptestpf17/sgdi_new/
+SQL instance: brsptestpf17\sqlserver2012
+db=CartaoVisita
+db=sgdi_new</t>
   </si>
 </sst>
 </file>
@@ -824,54 +834,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -892,6 +854,54 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1177,10 +1187,10 @@
   <dimension ref="A1:V21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T19" sqref="T19"/>
+      <selection pane="bottomRight" activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,11 +1338,11 @@
       <c r="R2" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="S2" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="T2" s="43" t="s">
         <v>134</v>
-      </c>
-      <c r="T2" s="59" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
@@ -1387,11 +1397,11 @@
       <c r="S3" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="T3" s="60" t="s">
-        <v>138</v>
+      <c r="T3" s="44" t="s">
+        <v>137</v>
       </c>
       <c r="U3" s="41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V3" s="32" t="s">
         <v>119</v>
@@ -1544,14 +1554,14 @@
       <c r="Q9" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="S9" s="61" t="s">
+      <c r="S9" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="T9" s="62" t="s">
-        <v>139</v>
+      <c r="T9" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="U9" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
@@ -1743,11 +1753,11 @@
       <c r="R13" s="36" t="s">
         <v>113</v>
       </c>
-      <c r="S13" s="63" t="s">
+      <c r="S13" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="T13" s="47" t="s">
         <v>144</v>
-      </c>
-      <c r="T13" s="63" t="s">
-        <v>145</v>
       </c>
       <c r="U13" s="38"/>
       <c r="V13" s="38"/>
@@ -1966,17 +1976,17 @@
       <c r="F18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S18" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="T18" s="64" t="s">
+      <c r="S18" s="42" t="s">
         <v>146</v>
       </c>
+      <c r="T18" s="48" t="s">
+        <v>145</v>
+      </c>
       <c r="U18" s="40" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1986,10 +1996,12 @@
       <c r="C19" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="S19" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="T19" s="65"/>
+      <c r="S19" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="T19" s="48" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
@@ -2004,8 +2016,8 @@
       <c r="S20" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="T20" s="65" t="s">
-        <v>143</v>
+      <c r="T20" s="49" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="45" x14ac:dyDescent="0.25">
@@ -2018,11 +2030,11 @@
       <c r="C21" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="S21" s="58" t="s">
+      <c r="S21" s="42" t="s">
+        <v>135</v>
+      </c>
+      <c r="T21" s="48" t="s">
         <v>136</v>
-      </c>
-      <c r="T21" s="64" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2076,22 +2088,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="57"/>
+      <c r="F1" s="55"/>
       <c r="G1" s="11" t="s">
         <v>62</v>
       </c>
@@ -2115,16 +2127,16 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="57"/>
+      <c r="F2" s="55"/>
       <c r="G2" s="11" t="s">
         <v>63</v>
       </c>
@@ -2148,23 +2160,23 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="49"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="51" t="s">
+      <c r="A3" s="63"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="52"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="55" t="s">
+      <c r="E3" s="51"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
-      <c r="L3" s="56"/>
-      <c r="M3" s="56"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2176,8 +2188,8 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="46"/>
-      <c r="E4" s="47"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="62"/>
       <c r="F4" s="16"/>
       <c r="G4" s="17"/>
       <c r="H4" s="1"/>
@@ -2197,8 +2209,8 @@
       <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="46"/>
-      <c r="E5" s="47"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="62"/>
       <c r="F5" s="16"/>
       <c r="G5" s="17"/>
       <c r="H5" s="1"/>
@@ -2212,20 +2224,20 @@
       <c r="A6" s="13"/>
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="52"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="55" t="s">
+      <c r="E6" s="51"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
-      <c r="J6" s="56"/>
-      <c r="K6" s="56"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="56"/>
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -2237,9 +2249,9 @@
       <c r="C7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="46"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="12"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -2258,9 +2270,9 @@
       <c r="C8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="57"/>
+      <c r="F8" s="57"/>
       <c r="G8" s="12"/>
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
@@ -2279,9 +2291,9 @@
       <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="46"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="12"/>
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
@@ -2300,9 +2312,9 @@
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="46"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="12"/>
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
@@ -2321,9 +2333,9 @@
       <c r="C11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="46"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
+      <c r="F11" s="57"/>
       <c r="G11" s="12"/>
       <c r="H11" s="1"/>
       <c r="I11" s="14"/>
@@ -2342,9 +2354,9 @@
       <c r="C12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="46"/>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="12"/>
       <c r="H12" s="14"/>
       <c r="I12" s="1"/>
@@ -2363,9 +2375,9 @@
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="46"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
       <c r="G13" s="12"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2384,9 +2396,9 @@
       <c r="C14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="46"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="54"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="57"/>
+      <c r="F14" s="57"/>
       <c r="G14" s="12"/>
       <c r="H14" s="1"/>
       <c r="I14" s="14"/>
@@ -2405,9 +2417,9 @@
       <c r="C15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="46"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="57"/>
       <c r="G15" s="12"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -2426,9 +2438,9 @@
       <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="46"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="57"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="12"/>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
@@ -2447,9 +2459,9 @@
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="46"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
       <c r="G17" s="12"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -2468,9 +2480,9 @@
       <c r="C18" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="46"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
       <c r="G18" s="18"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -2489,9 +2501,9 @@
       <c r="C19" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
       <c r="G19" s="18"/>
       <c r="H19" s="15"/>
       <c r="I19" s="15"/>
@@ -2510,9 +2522,9 @@
       <c r="C20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="46"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="54"/>
+      <c r="D20" s="56"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
       <c r="G20" s="12"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -2523,11 +2535,13 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="G3:M3"/>
-    <mergeCell ref="G6:M6"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
     <mergeCell ref="D19:F19"/>
     <mergeCell ref="D20:F20"/>
     <mergeCell ref="D7:F7"/>
@@ -2542,13 +2556,11 @@
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="D18:F18"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="G3:M3"/>
+    <mergeCell ref="G6:M6"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="E2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>